<commit_message>
web - config -commit
</commit_message>
<xml_diff>
--- a/doc/log/张非凡.xlsx
+++ b/doc/log/张非凡.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>时间段</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -235,6 +235,42 @@
   </si>
   <si>
     <t>完成student实体的构建并学习poi的基本操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.30  18：00-21：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对项目整体进行测试和改错</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.31  17：00-19：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.5   18：30-20：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习dispatcherservlet配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.6   18：30-20：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习一个简单的web的helloword例子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.7   16：30-18：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置web层的基本文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -657,10 +693,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -887,6 +923,46 @@
       </c>
       <c r="C27" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
614 commit for web controller
</commit_message>
<xml_diff>
--- a/doc/log/张非凡.xlsx
+++ b/doc/log/张非凡.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>时间段</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -271,6 +271,22 @@
   </si>
   <si>
     <t>配置web层的基本文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.11  18：00-20：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现json数据的返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.12  14：00-17：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习vue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -693,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -963,6 +979,22 @@
       </c>
       <c r="C32" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
618 commit for findlocation
</commit_message>
<xml_diff>
--- a/doc/log/张非凡.xlsx
+++ b/doc/log/张非凡.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>时间段</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -287,6 +287,10 @@
   </si>
   <si>
     <t>学习vue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.14</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -709,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -995,6 +999,11 @@
       </c>
       <c r="C34" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
623 commit for throne
</commit_message>
<xml_diff>
--- a/doc/log/张非凡.xlsx
+++ b/doc/log/张非凡.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>时间段</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -290,7 +290,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2019.6.14</t>
+    <t>2019.6.14  15：00-17：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习vue的基本模式和mvvm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.17  15：00-17：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>构建vue界面的基本框架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.18  18：00-20：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.20  18：00-20：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成对数据的CRUD操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习前后端的数据交互</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.19  14：00-17：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.21  20：00-22：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现数据交互，对tomcat和vue先后启动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现数据交互，对其进行完善</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -713,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1004,6 +1048,49 @@
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>68</v>
+      </c>
+      <c r="C35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
627 commit for over
</commit_message>
<xml_diff>
--- a/doc/log/张非凡.xlsx
+++ b/doc/log/张非凡.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="88">
   <si>
     <t>时间段</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,299 +42,331 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>2019.4.3   19：10-21：25</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.4.4   19：50-22.03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对jdbc进行学习，完成了jdbc测试中的连接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习jdbc中的statement connection prepared 事物概念 批量管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.4.7   11：30-12：30 18：21-19：21</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.4.8   20：20-21：40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习JPA创建时的前提设置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.4.10  20：30-22：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">配置hibernate到JPA中 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.4.11  17：50-20：22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>由于上次配置jpahelloword文件失败并且没有解决，重新配置了一个helloword文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.4.12  18：00-20：05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>注解，merge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.4.13  11：30-14:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>entitymanager,映射关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.4.16  21：00-22：47</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.4.29  18：30-20：18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对于sun工程进行配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.11  15：00-18：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查找contextconfiguration注解错误原因，写map相关内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.12  10：00-12：00 15：00-17：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对地点实体进行搭建，与地图实体构成多对一关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.13  19：00-21：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更改base层，dao层错误改为了对entitymanagerfactory无法调用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.14  16：30-17：30 20：00-21：12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更改dao层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.15  19：50-21：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.16  18：00-20：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重建项目的pom文件和git结构</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习xml的配置要素，重构了dao层和base层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.19  14：30-17：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将项目传送在git上进行协同开发使用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.20  15：30-17：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在eclipse上进行git的基本操作push，pull</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.22  13：00-14：50 16：30-18：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习分支的使用和git的基本使用流程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.21  10：30-11：50</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看dao层错误，寻找解决方法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.26  12：00-16：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>改正dao层错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.27  18：30-21：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>service层的实体管理器和方法的实现与测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.29  18：00-21：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成对学生表格的读取并存入数据库操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.28  13：44-17：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成student实体的构建并学习poi的基本操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.30  18：00-21：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对项目整体进行测试和改错</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.5.31  17：00-19：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.5   18：30-20：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习dispatcherservlet配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.6   18：30-20：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习一个简单的web的helloword例子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.7   16：30-18：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置web层的基本文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.11  18：00-20：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现json数据的返回</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.12  14：00-17：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习vue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.14  15：00-17：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习vue的基本模式和mvvm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.17  15：00-17：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>构建vue界面的基本框架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.18  18：00-20：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.20  18：00-20：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成对数据的CRUD操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习前后端的数据交互</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.19  14：00-17：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现数据交互，对tomcat和vue先后启动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现数据交互，对其进行完善</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.21  20：00-22：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.27  19：30-22：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改项目总体计划文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.26  13：30-15：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编写项目总体计划文档</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.25  19：00-21：00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改前后端交互代码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019.6.24  19：00-20：30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完善前端页面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>学习spring容器</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2019.4.3   19：10-21：25</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.4.4   19：50-22.03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对jdbc进行学习，完成了jdbc测试中的连接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习jdbc中的statement connection prepared 事物概念 批量管理</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.4.7   11：30-12：30 18：21-19：21</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>学习bolb，clob，时间处理，对jdbc连接操作、关闭操作打包</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.4.8   20：20-21：40</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习JPA创建时的前提设置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.4.10  20：30-22：30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">配置hibernate到JPA中 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.4.11  17：50-20：22</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>由于上次配置jpahelloword文件失败并且没有解决，重新配置了一个helloword文件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.4.12  18：00-20：05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>注解，merge</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.4.13  11：30-14:30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>entitymanager,映射关系</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.4.16  21：00-22：47</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>dao</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.4.29  18：30-20：18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对于sun工程进行配置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.11  15：00-18：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查找contextconfiguration注解错误原因，写map相关内容</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.12  10：00-12：00 15：00-17：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对地点实体进行搭建，与地图实体构成多对一关系</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.13  19：00-21：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>更改base层，dao层错误改为了对entitymanagerfactory无法调用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.14  16：30-17：30 20：00-21：12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>更改dao层</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.15  19：50-21：30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.16  18：00-20：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重建项目的pom文件和git结构</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习xml的配置要素，重构了dao层和base层</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.19  14：30-17：30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>将项目传送在git上进行协同开发使用</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.20  15：30-17：30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在eclipse上进行git的基本操作push，pull</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.22  13：00-14：50 16：30-18：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习分支的使用和git的基本使用流程</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.21  10：30-11：50</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>查看dao层错误，寻找解决方法</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.26  12：00-16：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>改正dao层错误</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.27  18：30-21：30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>service层的实体管理器和方法的实现与测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.29  18：00-21：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成对学生表格的读取并存入数据库操作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.28  13：44-17：30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成student实体的构建并学习poi的基本操作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.30  18：00-21：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>对项目整体进行测试和改错</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.5.31  17：00-19：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.5   18：30-20：30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习dispatcherservlet配置</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.6   18：30-20：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习一个简单的web的helloword例子</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.7   16：30-18：30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>配置web层的基本文件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.11  18：00-20：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>实现json数据的返回</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.12  14：00-17：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习vue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.14  15：00-17：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习vue的基本模式和mvvm</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.17  15：00-17：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>构建vue界面的基本框架</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.18  18：00-20：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.20  18：00-20：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成对数据的CRUD操作</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学习前后端的数据交互</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.19  14：00-17：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2019.6.21  20：00-22：00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>实现数据交互，对tomcat和vue先后启动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>实现数据交互，对其进行完善</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -757,10 +789,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -794,295 +826,295 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
         <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
         <v>36</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -1090,7 +1122,39 @@
         <v>77</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>82</v>
+      </c>
+      <c r="C42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>